<commit_message>
# Expressed gene list more presentable
</commit_message>
<xml_diff>
--- a/lists/bottom_pen.xlsx
+++ b/lists/bottom_pen.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,42 +360,22 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Parent</t>
+          <t>GeneID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>baseMean</t>
+          <t>log2FoldChange</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>log2FoldChange</t>
+          <t>padj</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>lfcSE</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>stat</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>pvalue</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>padj</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Note</t>
+          <t>Hypthetical Function</t>
         </is>
       </c>
     </row>
@@ -406,24 +386,12 @@
         </is>
       </c>
       <c r="B2">
-        <v>28.176911195908</v>
+        <v>-7.219425348559308</v>
       </c>
       <c r="C2">
-        <v>-7.219425348559308</v>
-      </c>
-      <c r="D2">
-        <v>1.412084245041446</v>
-      </c>
-      <c r="E2">
-        <v>-5.112602434245991</v>
-      </c>
-      <c r="F2">
-        <v>3.177505812012812e-007</v>
-      </c>
-      <c r="G2">
         <v>2.77280487797118e-006</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>GNS1/SUR4 membrane protein family | FUNCTIONS IN: molecular_function unknown | INVOLVED IN: biological_process unknown | LOCATED IN: integral to membrane | EXPRESSED IN: root | CONTAINS InterPro DOMAIN/s: GNS1/SUR4 membrane protein | BEST Arabidopsis thaliana protein match is: GNS1/SUR4 membrane protein family</t>
         </is>
@@ -436,24 +404,12 @@
         </is>
       </c>
       <c r="B3">
-        <v>51.55745602671088</v>
+        <v>-7.203099695623153</v>
       </c>
       <c r="C3">
-        <v>-7.203099695623153</v>
-      </c>
-      <c r="D3">
-        <v>1.177940261234807</v>
-      </c>
-      <c r="E3">
-        <v>-6.114995753750968</v>
-      </c>
-      <c r="F3">
-        <v>9.655953467756452e-010</v>
-      </c>
-      <c r="G3">
         <v>1.24154275484334e-008</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>putative beta-expansin/allergen protein. Naming convention from the Expansin Working Group (Kende et al, 2004. Plant Mol Bio). Involved in the formation of nematode-induced syncytia in roots of Arabidopsis thaliana. | expansin B3 (EXPB3) | INVOLVED IN: response to cyclopentenone, syncytium formation, plant-type cell wall organization, unidimensional cell growth, plant-type cell wall loosening | LOCATED IN: endomembrane system, extracellular region | EXPRESSED IN: 21 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Barwin-related endoglucanase , Pollen allergen, N-terminal , Rare lipoprotein A , Major pollen allergen Lol pI , Expansin/Lol pI , Expansin 45, endoglucanase-like , Pollen allergen/expansin, C-terminal | BEST Arabidopsis thaliana protein match is: expansin B1</t>
         </is>
@@ -466,24 +422,12 @@
         </is>
       </c>
       <c r="B4">
-        <v>8.786632190149058</v>
+        <v>-6.507419428501581</v>
       </c>
       <c r="C4">
-        <v>-6.507419428501581</v>
-      </c>
-      <c r="D4">
-        <v>1.436069517598984</v>
-      </c>
-      <c r="E4">
-        <v>-4.531409760289021</v>
-      </c>
-      <c r="F4">
-        <v>5.859136472819956e-006</v>
-      </c>
-      <c r="G4">
         <v>4.010720539649392e-005</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>IQ-domain 18 (IQD18) | FUNCTIONS IN: molecular_function unknown | EXPRESSED IN: 10 plant structures | EXPRESSED DURING: 6 growth stages | CONTAINS InterPro DOMAIN/s: IQ calmodulin-binding region | BEST Arabidopsis thaliana protein match is: IQ-domain 17</t>
         </is>
@@ -496,24 +440,12 @@
         </is>
       </c>
       <c r="B5">
-        <v>16.49736487769551</v>
+        <v>-6.44071810642849</v>
       </c>
       <c r="C5">
-        <v>-6.44071810642849</v>
-      </c>
-      <c r="D5">
-        <v>1.331763332982711</v>
-      </c>
-      <c r="E5">
-        <v>-4.836233245739995</v>
-      </c>
-      <c r="F5">
-        <v>1.323226433914024e-006</v>
-      </c>
-      <c r="G5">
         <v>1.034054839748016e-005</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Leucine-rich receptor-like protein kinase family protein | FUNCTIONS IN: protein serine/threonine kinase activity, kinase activity, ATP binding | INVOLVED IN: transmembrane receptor protein tyrosine kinase signaling pathway, protein amino acid phosphorylation | LOCATED IN: plasma membrane | EXPRESSED IN: 21 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Protein kinase, catalytic domain , Leucine-rich repeat-containing N-terminal domain, type 2 , Leucine-rich repeat , Serine-threonine/tyrosine-protein kinase , Protein kinase-like domain , Serine/threonine-protein kinase, active site | BEST Arabidopsis thaliana protein match is: Leucine-rich receptor-like protein kinase family protein</t>
         </is>
@@ -526,24 +458,12 @@
         </is>
       </c>
       <c r="B6">
-        <v>26.74173985277654</v>
+        <v>-6.274495086062387</v>
       </c>
       <c r="C6">
-        <v>-6.274495086062387</v>
-      </c>
-      <c r="D6">
-        <v>1.125022503516594</v>
-      </c>
-      <c r="E6">
-        <v>-5.577217403607106</v>
-      </c>
-      <c r="F6">
-        <v>2.443963572861249e-008</v>
-      </c>
-      <c r="G6">
         <v>2.554475203314678e-007</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>unknown protein | FUNCTIONS IN: molecular_function unknown | INVOLVED IN: biological_process unknown | LOCATED IN: plasma membrane | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 13 growth stages</t>
         </is>
@@ -556,24 +476,12 @@
         </is>
       </c>
       <c r="B7">
-        <v>1238.523923429605</v>
+        <v>-6.232968957116001</v>
       </c>
       <c r="C7">
-        <v>-6.232968957116001</v>
-      </c>
-      <c r="D7">
-        <v>0.2586400489238453</v>
-      </c>
-      <c r="E7">
-        <v>-24.0990093492878</v>
-      </c>
-      <c r="F7">
-        <v>2.560210503876214e-128</v>
-      </c>
-      <c r="G7">
         <v>1.921352642808969e-124</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>encodes a beta-mannan synthase based on in vitro enzyme assays from heterologously expressed protein | cellulose synthase-like A02 (CSLA02) | CONTAINS InterPro DOMAIN/s: Glycosyl transferase, family 2 | BEST Arabidopsis thaliana protein match is: Nucleotide-diphospho-sugar transferases superfamily protein</t>
         </is>
@@ -586,24 +494,12 @@
         </is>
       </c>
       <c r="B8">
-        <v>6.787918119997301</v>
+        <v>-6.136186703771024</v>
       </c>
       <c r="C8">
-        <v>-6.136186703771024</v>
-      </c>
-      <c r="D8">
-        <v>1.500974228510789</v>
-      </c>
-      <c r="E8">
-        <v>-4.088135950114961</v>
-      </c>
-      <c r="F8">
-        <v>4.348533004210067e-005</v>
-      </c>
-      <c r="G8">
         <v>0.0002454936611253396</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Cyclin B2, 3 (CYCB2, 3) | FUNCTIONS IN: cyclin-dependent protein kinase regulator activity | INVOLVED IN: regulation of cell cycle | LOCATED IN: nucleus | CONTAINS InterPro DOMAIN/s: Cyclin, C-terminal , Cyclin-like , Cyclin-related , Cyclin, N-terminal , Cyclin, A/B/D/E , Cyclin | BEST Arabidopsis thaliana protein match is: CYCLIN B2, 4</t>
         </is>
@@ -616,24 +512,12 @@
         </is>
       </c>
       <c r="B9">
-        <v>6.787980151498391</v>
+        <v>-6.135530831738205</v>
       </c>
       <c r="C9">
-        <v>-6.135530831738205</v>
-      </c>
-      <c r="D9">
-        <v>1.667132913228073</v>
-      </c>
-      <c r="E9">
-        <v>-3.680288945803345</v>
-      </c>
-      <c r="F9">
-        <v>0.0002329698156982867</v>
-      </c>
-      <c r="G9">
         <v>0.00108774003123833</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Glucan endo-1,3-beta-glucosidase, acidic isoform GI9 precursor (EC 3.2.1.39) ((1- 3)-beta-glucan endohydrolase) ((1- 3)-beta-glucanase) (Beta-1,3-endoglucanase) (PR-2B) (PR-36) - Nicotiana tabacum (Common tobacco), Glycosyl hydrolase superfamily protein | FUNCTIONS IN: cation binding, hydrolase activity, hydrolyzing O-glycosyl compounds, catalytic activity | INVOLVED IN: defense response to fungus, incompatible interaction, response to salt stress | LOCATED IN: cell wall, plasma membrane | EXPRESSED IN: 11 plant structures | EXPRESSED DURING: LP.06 six leaves visible, LP.04 four leaves visible, 4 anthesis, petal differentiation and expansion stage, LP.08 eight leaves visible | CONTAINS InterPro DOMAIN/s: Glycoside hydrolase, catalytic core , Glycoside hydrolase, family 17 , Glycoside hydrolase, subgroup, catalytic core | BEST Arabidopsis thaliana protein match is: beta-1,3-glucanase 1</t>
         </is>
@@ -646,24 +530,12 @@
         </is>
       </c>
       <c r="B10">
-        <v>79.75873191619078</v>
+        <v>-6.098612123438509</v>
       </c>
       <c r="C10">
-        <v>-6.098612123438509</v>
-      </c>
-      <c r="D10">
-        <v>1.239245130908375</v>
-      </c>
-      <c r="E10">
-        <v>-4.92123145883832</v>
-      </c>
-      <c r="F10">
-        <v>8.600134730529997e-007</v>
-      </c>
-      <c r="G10">
         <v>6.932453753066679e-006</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -676,24 +548,12 @@
         </is>
       </c>
       <c r="B11">
-        <v>36.27393264845294</v>
+        <v>-6.08411422895832</v>
       </c>
       <c r="C11">
-        <v>-6.08411422895832</v>
-      </c>
-      <c r="D11">
-        <v>0.9245518248705299</v>
-      </c>
-      <c r="E11">
-        <v>-6.580609183060465</v>
-      </c>
-      <c r="F11">
-        <v>4.685246283352453e-011</v>
-      </c>
-      <c r="G11">
         <v>7.103275072282635e-010</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>beta-galactosidase 16 (BGAL16) | FUNCTIONS IN: cation binding, sugar binding, beta-galactosidase activity, hydrolase activity, hydrolyzing O-glycosyl compounds, catalytic activity | INVOLVED IN: lactose catabolic process, using glucoside 3-dehydrogenase, carbohydrate metabolic process, lactose catabolic process via UDP-galactose, lactose catabolic process | LOCATED IN: endomembrane system | EXPRESSED IN: 27 plant structures | EXPRESSED DURING: 15 growth stages | CONTAINS InterPro DOMAIN/s: Glycoside hydrolase, family 35, conserved site , Glycoside hydrolase, family 35 , D-galactoside/L-rhamnose binding SUEL lectin , Glycoside hydrolase, catalytic core , Glycoside hydrolase, subgroup, catalytic core , Galactose-binding domain-like | BEST Arabidopsis thaliana protein match is: Glycosyl hydrolase family 35 protein</t>
         </is>
@@ -706,24 +566,12 @@
         </is>
       </c>
       <c r="B12">
-        <v>11.38346392532984</v>
+        <v>-5.90227764200551</v>
       </c>
       <c r="C12">
-        <v>-5.90227764200551</v>
-      </c>
-      <c r="D12">
-        <v>1.379856668435389</v>
-      </c>
-      <c r="E12">
-        <v>-4.27745705552017</v>
-      </c>
-      <c r="F12">
-        <v>1.890404119755846e-005</v>
-      </c>
-      <c r="G12">
         <v>0.0001161587291271374</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Major facilitator superfamily protein | FUNCTIONS IN: tetracycline transporter activity | INVOLVED IN: response to antibiotic, tetracycline transport, transmembrane transport | LOCATED IN: endomembrane system, integral to membrane | EXPRESSED IN: 6 plant structures | EXPRESSED DURING: L mature pollen stage, 4 anthesis | CONTAINS InterPro DOMAIN/s: Tetracycline resistance protein, TetA , Major facilitator superfamily MFS-1 , Major facilitator superfamily, general substrate transporter | BEST Arabidopsis thaliana protein match is: Major facilitator superfamily protein</t>
         </is>
@@ -736,24 +584,12 @@
         </is>
       </c>
       <c r="B13">
-        <v>5.492305737563556</v>
+        <v>-5.84041299400148</v>
       </c>
       <c r="C13">
-        <v>-5.84041299400148</v>
-      </c>
-      <c r="D13">
-        <v>1.477487866778892</v>
-      </c>
-      <c r="E13">
-        <v>-3.952934657077291</v>
-      </c>
-      <c r="F13">
-        <v>7.719852370638158e-005</v>
-      </c>
-      <c r="G13">
         <v>0.0004071322470661689</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -766,24 +602,12 @@
         </is>
       </c>
       <c r="B14">
-        <v>4.991660717014077</v>
+        <v>-5.690229211154548</v>
       </c>
       <c r="C14">
-        <v>-5.690229211154548</v>
-      </c>
-      <c r="D14">
-        <v>1.706709865210515</v>
-      </c>
-      <c r="E14">
-        <v>-3.334034288512584</v>
-      </c>
-      <c r="F14">
-        <v>0.0008559610536387731</v>
-      </c>
-      <c r="G14">
         <v>0.003428412588796182</v>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>myb-like transcription factor family protein | CONTAINS InterPro DOMAIN/s: SANT, DNA-binding , Homeodomain-like , Myb, DNA-binding , Zinc finger, CCHC-type , HTH transcriptional regulator, Myb-type, DNA-binding , Myb-like DNA-binding domain, SHAQKYF class | BEST Arabidopsis thaliana protein match is: Homeodomain-like superfamily protein</t>
         </is>
@@ -796,24 +620,12 @@
         </is>
       </c>
       <c r="B15">
-        <v>305.1840384520393</v>
+        <v>-5.683268589119459</v>
       </c>
       <c r="C15">
-        <v>-5.683268589119459</v>
-      </c>
-      <c r="D15">
-        <v>0.3121013034370281</v>
-      </c>
-      <c r="E15">
-        <v>-18.20969193826567</v>
-      </c>
-      <c r="F15">
-        <v>4.323727894049704e-074</v>
-      </c>
-      <c r="G15">
         <v>3.605348511356853e-071</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>fasciclin-like arabinogalactan-protein 1 (Fla1) | FASCICLIN-like arabinogalactan 1 (FLA1) | CONTAINS InterPro DOMAIN/s: FAS1 domain | BEST Arabidopsis thaliana protein match is: FASCICLIN-like arabinogalactan 2 .</t>
         </is>
@@ -826,24 +638,12 @@
         </is>
       </c>
       <c r="B16">
-        <v>9.700554747183496</v>
+        <v>-5.679778558270267</v>
       </c>
       <c r="C16">
-        <v>-5.679778558270267</v>
-      </c>
-      <c r="D16">
-        <v>1.450880282212683</v>
-      </c>
-      <c r="E16">
-        <v>-3.914712073699321</v>
-      </c>
-      <c r="F16">
-        <v>9.051215262596219e-005</v>
-      </c>
-      <c r="G16">
         <v>0.0004696452187649027</v>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Zinc-binding dehydrogenase family protein | FUNCTIONS IN: oxidoreductase activity, binding, zinc ion binding, catalytic activity | INVOLVED IN: oxidation reduction, metabolic process | LOCATED IN: cellular_component unknown | EXPRESSED IN: 23 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: GroES-like , NAD(P)-binding domain , Alcohol dehydrogenase, C-terminal , Alcohol dehydrogenase superfamily, zinc-containing | BEST Arabidopsis thaliana protein match is: alkenal reductase</t>
         </is>
@@ -856,24 +656,12 @@
         </is>
       </c>
       <c r="B17">
-        <v>80.29114915146151</v>
+        <v>-5.660240660789782</v>
       </c>
       <c r="C17">
-        <v>-5.660240660789782</v>
-      </c>
-      <c r="D17">
-        <v>0.585051367554546</v>
-      </c>
-      <c r="E17">
-        <v>-9.674775540563216</v>
-      </c>
-      <c r="F17">
-        <v>3.85937602013693e-022</v>
-      </c>
-      <c r="G17">
         <v>1.758906714926373e-020</v>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>glycosyl hydrolase 9B13 (GH9B13) | FUNCTIONS IN: hydrolase activity, hydrolyzing O-glycosyl compounds, catalytic activity | INVOLVED IN: carbohydrate metabolic process | LOCATED IN: endomembrane system | EXPRESSED IN: 20 plant structures | EXPRESSED DURING: 9 growth stages | CONTAINS InterPro DOMAIN/s: Six-hairpin glycosidase , Glycoside hydrolase, family 9, active site , Six-hairpin glycosidase-like , Glycoside hydrolase, family 9 | BEST Arabidopsis thaliana protein match is: cellulase 2</t>
         </is>
@@ -886,24 +674,12 @@
         </is>
       </c>
       <c r="B18">
-        <v>4.810029857109607</v>
+        <v>-5.653738725259677</v>
       </c>
       <c r="C18">
-        <v>-5.653738725259677</v>
-      </c>
-      <c r="D18">
-        <v>1.642798622378312</v>
-      </c>
-      <c r="E18">
-        <v>-3.441528771843409</v>
-      </c>
-      <c r="F18">
-        <v>0.0005784369521734411</v>
-      </c>
-      <c r="G18">
         <v>0.002422683735201069</v>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -916,24 +692,12 @@
         </is>
       </c>
       <c r="B19">
-        <v>35.27566793983153</v>
+        <v>-5.632390168629408</v>
       </c>
       <c r="C19">
-        <v>-5.632390168629408</v>
-      </c>
-      <c r="D19">
-        <v>0.8811968090019379</v>
-      </c>
-      <c r="E19">
-        <v>-6.391750527341074</v>
-      </c>
-      <c r="F19">
-        <v>1.639973105831891e-010</v>
-      </c>
-      <c r="G19">
         <v>2.332429216974049e-009</v>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Zeatin O-xylosyltransferase (EC 2.4.2.40) (Zeatin O-beta-D-xylosyltransferase) - Phaseolus vulgaris (Kidney bean) (French bean), UDP-Glycosyltransferase superfamily protein | FUNCTIONS IN: UDP-glycosyltransferase activity, transferase activity, transferring glycosyl groups | INVOLVED IN: metabolic process | LOCATED IN: cellular_component unknown | EXPRESSED IN: embryo, sepal, flower, pedicel, synergid | EXPRESSED DURING: 4 anthesis, C globular stage | CONTAINS InterPro DOMAIN/s: UDP-glucuronosyl/UDP-glucosyltransferase | BEST Arabidopsis thaliana protein match is: UDP-glucosyl transferase 72E1</t>
         </is>
@@ -946,24 +710,12 @@
         </is>
       </c>
       <c r="B20">
-        <v>4.767226042967149</v>
+        <v>-5.625282102791512</v>
       </c>
       <c r="C20">
-        <v>-5.625282102791512</v>
-      </c>
-      <c r="D20">
-        <v>1.717432798126674</v>
-      </c>
-      <c r="E20">
-        <v>-3.275401581318004</v>
-      </c>
-      <c r="F20">
-        <v>0.001055118710579606</v>
-      </c>
-      <c r="G20">
         <v>0.00411412238482668</v>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>homeobox protein 31 (HB31) | FUNCTIONS IN: DNA binding, sequence-specific DNA binding transcription factor activity | INVOLVED IN: regulation of transcription | LOCATED IN: cellular_component unknown | EXPRESSED IN: 17 plant structures | EXPRESSED DURING: 11 growth stages | CONTAINS InterPro DOMAIN/s: Homeobox domain, ZF-HD class , ZF-HD homeobox protein, Cys/His-rich dimerisation domain , Homeodomain-related | BEST Arabidopsis thaliana protein match is: homeobox protein 21</t>
         </is>
@@ -976,24 +728,12 @@
         </is>
       </c>
       <c r="B21">
-        <v>9.340509482789519</v>
+        <v>-5.601173963494664</v>
       </c>
       <c r="C21">
-        <v>-5.601173963494664</v>
-      </c>
-      <c r="D21">
-        <v>1.599126020919894</v>
-      </c>
-      <c r="E21">
-        <v>-3.5026470023123</v>
-      </c>
-      <c r="F21">
-        <v>0.0004606595122183066</v>
-      </c>
-      <c r="G21">
         <v>0.001984555732507263</v>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -1006,24 +746,12 @@
         </is>
       </c>
       <c r="B22">
-        <v>67.54621228139442</v>
+        <v>-5.576926010772976</v>
       </c>
       <c r="C22">
-        <v>-5.576926010772976</v>
-      </c>
-      <c r="D22">
-        <v>0.6870354381624946</v>
-      </c>
-      <c r="E22">
-        <v>-8.117377504847058</v>
-      </c>
-      <c r="F22">
-        <v>4.763652214805757e-016</v>
-      </c>
-      <c r="G22">
         <v>1.2662203773806e-014</v>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>GDSL-like Lipase/Acylhydrolase superfamily protein | FUNCTIONS IN: hydrolase activity, acting on ester bonds, carboxylesterase activity | INVOLVED IN: glycerol biosynthetic process, lipid metabolic process | LOCATED IN: endomembrane system | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 14 growth stages | CONTAINS InterPro DOMAIN/s: Lipase, GDSL | BEST Arabidopsis thaliana protein match is: GDSL-like Lipase/Acylhydrolase superfamily protein</t>
         </is>
@@ -1036,24 +764,12 @@
         </is>
       </c>
       <c r="B23">
-        <v>4.418946897149301</v>
+        <v>-5.527314577730581</v>
       </c>
       <c r="C23">
-        <v>-5.527314577730581</v>
-      </c>
-      <c r="D23">
-        <v>1.510942769579355</v>
-      </c>
-      <c r="E23">
-        <v>-3.658189237220006</v>
-      </c>
-      <c r="F23">
-        <v>0.0002540034796772072</v>
-      </c>
-      <c r="G23">
         <v>0.001172812621298737</v>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Major facilitator superfamily protein | FUNCTIONS IN: carbohydrate transmembrane transporter activity, sugar:hydrogen symporter activity | INVOLVED IN: transport, transmembrane transport | LOCATED IN: integral to membrane, membrane | EXPRESSED IN: 19 plant structures | EXPRESSED DURING: 10 growth stages | CONTAINS InterPro DOMAIN/s: Sugar transporter, conserved site , Major facilitator superfamily , General substrate transporter , Sugar/inositol transporter , Major facilitator superfamily, general substrate transporter | BEST Arabidopsis thaliana protein match is: Major facilitator superfamily protein</t>
         </is>
@@ -1066,24 +782,12 @@
         </is>
       </c>
       <c r="B24">
-        <v>8.832027051752643</v>
+        <v>-5.523179740565047</v>
       </c>
       <c r="C24">
-        <v>-5.523179740565047</v>
-      </c>
-      <c r="D24">
-        <v>1.395281325815166</v>
-      </c>
-      <c r="E24">
-        <v>-3.958470337398258</v>
-      </c>
-      <c r="F24">
-        <v>7.54313067353162e-005</v>
-      </c>
-      <c r="G24">
         <v>0.0003997788229375963</v>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>fasciclin-like arabinogalactan-protein 9 (Fla9) | FASCICLIN-like arabinoogalactan 9 (FLA9) | LOCATED IN: anchored to plasma membrane, plasma membrane, anchored to membrane | EXPRESSED IN: 23 plant structures | EXPRESSED DURING: 14 growth stages | CONTAINS InterPro DOMAIN/s: FAS1 domain | BEST Arabidopsis thaliana protein match is: FASCICLIN-like arabinogalactan protein 13 precursor</t>
         </is>
@@ -1096,24 +800,12 @@
         </is>
       </c>
       <c r="B25">
-        <v>8.537722462206425</v>
+        <v>-5.472557402424445</v>
       </c>
       <c r="C25">
-        <v>-5.472557402424445</v>
-      </c>
-      <c r="D25">
-        <v>1.351295864959558</v>
-      </c>
-      <c r="E25">
-        <v>-4.049858764711182</v>
-      </c>
-      <c r="F25">
-        <v>5.124855368797737e-005</v>
-      </c>
-      <c r="G25">
         <v>0.0002839099256228155</v>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -1126,24 +818,12 @@
         </is>
       </c>
       <c r="B26">
-        <v>39.30190578894656</v>
+        <v>-5.465293811660585</v>
       </c>
       <c r="C26">
-        <v>-5.465293811660585</v>
-      </c>
-      <c r="D26">
-        <v>0.797322400475853</v>
-      </c>
-      <c r="E26">
-        <v>-6.854559471048126</v>
-      </c>
-      <c r="F26">
-        <v>7.153260859921645e-012</v>
-      </c>
-      <c r="G26">
         <v>1.198277641371101e-010</v>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Remorin family protein | FUNCTIONS IN: DNA binding | INVOLVED IN: biological_process unknown | LOCATED IN: nucleus | EXPRESSED IN: 23 plant structures | EXPRESSED DURING: 12 growth stages | CONTAINS InterPro DOMAIN/s: Remorin, C-terminal | BEST Arabidopsis thaliana protein match is: Remorin family protein</t>
         </is>
@@ -1156,24 +836,12 @@
         </is>
       </c>
       <c r="B27">
-        <v>46.4056117471595</v>
+        <v>-5.436682778618221</v>
       </c>
       <c r="C27">
-        <v>-5.436682778618221</v>
-      </c>
-      <c r="D27">
-        <v>0.7635669247686348</v>
-      </c>
-      <c r="E27">
-        <v>-7.120112988479127</v>
-      </c>
-      <c r="F27">
-        <v>1.078386230904461e-012</v>
-      </c>
-      <c r="G27">
         <v>2.016510598221182e-011</v>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Encodes a member of the TBL (TRICHOME BIREFRINGENCE-LIKE) gene family containing a plant-specific DUF231 (domain of unknown function) domain. TBL gene family has 46 members, two of which (TBR/AT5G06700 and TBL3/AT5G01360) have been shown to be involved in the synthesis and deposition of secondary wall cellulose, presumably by influencing the esterification state of pectic polymers. A nomenclature for this gene family has been proposed (Volker Bischoff, Wolf Scheible, 2010, personal communication). | TRICHOME BIREFRINGENCE-LIKE 41 (TBL41) | INVOLVED IN: biological_process unknown | LOCATED IN: endomembrane system | EXPRESSED IN: 11 plant structures | EXPRESSED DURING: 4 anthesis, C globular stage, petal differentiation and expansion stage | CONTAINS InterPro DOMAIN/s: Protein of unknown function DUF231, plant | BEST Arabidopsis thaliana protein match is: TRICHOME BIREFRINGENCE-LIKE 38</t>
         </is>
@@ -1186,24 +854,12 @@
         </is>
       </c>
       <c r="B28">
-        <v>45.01569711673475</v>
+        <v>-5.390518922559171</v>
       </c>
       <c r="C28">
-        <v>-5.390518922559171</v>
-      </c>
-      <c r="D28">
-        <v>0.6913745489408978</v>
-      </c>
-      <c r="E28">
-        <v>-7.796814231615546</v>
-      </c>
-      <c r="F28">
-        <v>6.348959792187732e-015</v>
-      </c>
-      <c r="G28">
         <v>1.515805734478416e-013</v>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>protein serine/threonine kinases, protein kinases, ATP binding, sugar binding, kinases, carbohydrate binding | FUNCTIONS IN: in 6 functions | INVOLVED IN: protein amino acid phosphorylation, recognition of pollen | LOCATED IN: endomembrane system | EXPRESSED IN: 12 plant structures | EXPRESSED DURING: 6 growth stages | CONTAINS InterPro DOMAIN/s: Curculin-like (mannose-binding) lectin , Apple-like , PAN-2 domain , Serine/threonine-protein kinase domain , Serine-threonine/tyrosine-protein kinase , Serine/threonine-protein kinase-like domain , Protein kinase-like domain , Serine/threonine-protein kinase, active site , Protein kinase, catalytic domain , S-locus glycoprotein , Tyrosine-protein kinase, catalytic domain | BEST Arabidopsis thaliana protein match is: S-locus lectin protein kinase family protein</t>
         </is>
@@ -1216,24 +872,12 @@
         </is>
       </c>
       <c r="B29">
-        <v>22.46152409137023</v>
+        <v>-5.390309761751656</v>
       </c>
       <c r="C29">
-        <v>-5.390309761751656</v>
-      </c>
-      <c r="D29">
-        <v>0.9435218174111415</v>
-      </c>
-      <c r="E29">
-        <v>-5.712967800301344</v>
-      </c>
-      <c r="F29">
-        <v>1.110226927811004e-008</v>
-      </c>
-      <c r="G29">
         <v>1.223477682463874e-007</v>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -1246,24 +890,12 @@
         </is>
       </c>
       <c r="B30">
-        <v>28.91489985206725</v>
+        <v>-5.352298158138244</v>
       </c>
       <c r="C30">
-        <v>-5.352298158138244</v>
-      </c>
-      <c r="D30">
-        <v>0.8169372133169125</v>
-      </c>
-      <c r="E30">
-        <v>-6.551664033527066</v>
-      </c>
-      <c r="F30">
-        <v>5.689944017354649e-011</v>
-      </c>
-      <c r="G30">
         <v>8.517513271723575e-010</v>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>ROP interactive partner 3 (RIP3) | LOCATED IN: chloroplast | EXPRESSED IN: 21 plant structures | EXPRESSED DURING: 12 growth stages | BEST Arabidopsis thaliana protein match is: ROP interactive partner 4</t>
         </is>
@@ -1276,24 +908,12 @@
         </is>
       </c>
       <c r="B31">
-        <v>14.98420843668827</v>
+        <v>-5.334637546478382</v>
       </c>
       <c r="C31">
-        <v>-5.334637546478382</v>
-      </c>
-      <c r="D31">
-        <v>1.230304489858445</v>
-      </c>
-      <c r="E31">
-        <v>-4.336030300183794</v>
-      </c>
-      <c r="F31">
-        <v>1.450789540360352e-005</v>
-      </c>
-      <c r="G31">
         <v>9.172444737903106e-005</v>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>UDP-glucose:indole-3-acetate beta-D-glucosyltransferase | indole-3-acetate beta-D-glucosyltransferase (IAGLU) | FUNCTIONS IN: UDP-glycosyltransferase activity, transferase activity, transferring glycosyl groups | INVOLVED IN: metabolic process | LOCATED IN: chloroplast | EXPRESSED IN: 17 plant structures | EXPRESSED DURING: 7 growth stages | CONTAINS InterPro DOMAIN/s: UDP-glucuronosyl/UDP-glucosyltransferase | BEST Arabidopsis thaliana protein match is: UDP-glucosyltransferase 75B1</t>
         </is>
@@ -1306,24 +926,12 @@
         </is>
       </c>
       <c r="B32">
-        <v>105.4309891108851</v>
+        <v>-5.24269057459525</v>
       </c>
       <c r="C32">
-        <v>-5.24269057459525</v>
-      </c>
-      <c r="D32">
-        <v>0.6148526300658457</v>
-      </c>
-      <c r="E32">
-        <v>-8.526743349920778</v>
-      </c>
-      <c r="F32">
-        <v>1.505253261289028e-017</v>
-      </c>
-      <c r="G32">
         <v>4.623365883309847e-016</v>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Plant invertase/pectin methylesterase inhibitor superfamily protein | FUNCTIONS IN: enzyme inhibitor activity, pectinesterase inhibitor activity, pectinesterase activity | INVOLVED IN: biological_process unknown | LOCATED IN: cellular_component unknown | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Pectinesterase inhibitor | BEST Arabidopsis thaliana protein match is: Plant invertase/pectin methylesterase inhibitor superfamily protein</t>
         </is>
@@ -1336,24 +944,12 @@
         </is>
       </c>
       <c r="B33">
-        <v>3.625441892384818</v>
+        <v>-5.231286182310262</v>
       </c>
       <c r="C33">
-        <v>-5.231286182310262</v>
-      </c>
-      <c r="D33">
-        <v>2.005145053571989</v>
-      </c>
-      <c r="E33">
-        <v>-2.608931544873118</v>
-      </c>
-      <c r="F33">
-        <v>0.009082540961081334</v>
-      </c>
-      <c r="G33">
         <v>0.02643624139596447</v>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Putative transcription factor with zinc finger and helix-loop-helix domains, the later similar to HMG boxes. Involved in specifying abaxial cell fate in the carpel. Four putative LFY binding sites (CCANTG) and two potential binding sites for MADS box proteins known as CArG boxes (CC(A/T)6GG) were found in the region spanning 3.8 Kb upstream of the CRC coding region. | CRABS CLAW (CRC) | CONTAINS InterPro DOMAIN/s: High mobility group, superfamily , YABBY protein | BEST Arabidopsis thaliana protein match is: Plant-specific transcription factor YABBY family protein</t>
         </is>
@@ -1366,24 +962,12 @@
         </is>
       </c>
       <c r="B34">
-        <v>3.609040380676723</v>
+        <v>-5.225254393659978</v>
       </c>
       <c r="C34">
-        <v>-5.225254393659978</v>
-      </c>
-      <c r="D34">
-        <v>2.015390528985067</v>
-      </c>
-      <c r="E34">
-        <v>-2.592675870264891</v>
-      </c>
-      <c r="F34">
-        <v>0.009523247620060019</v>
-      </c>
-      <c r="G34">
         <v>0.02754096299525129</v>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>unknown protein | BEST Arabidopsis thaliana protein match is: unknown protein</t>
         </is>
@@ -1396,24 +980,12 @@
         </is>
       </c>
       <c r="B35">
-        <v>3.460912706997789</v>
+        <v>-5.168071317556493</v>
       </c>
       <c r="C35">
-        <v>-5.168071317556493</v>
-      </c>
-      <c r="D35">
-        <v>1.589372452899917</v>
-      </c>
-      <c r="E35">
-        <v>-3.251642689620675</v>
-      </c>
-      <c r="F35">
-        <v>0.001147401658313994</v>
-      </c>
-      <c r="G35">
         <v>0.004432706396167082</v>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>inosine-uridine preferring nucleoside hydrolase family protein | FUNCTIONS IN: hydrolase activity | INVOLVED IN: biological_process unknown | LOCATED IN: cell wall | CONTAINS InterPro DOMAIN/s: Inosine/uridine-preferring nucleoside hydrolase | BEST Arabidopsis thaliana protein match is: Inosine-uridine preferring nucleoside hydrolase family protein</t>
         </is>
@@ -1426,24 +998,12 @@
         </is>
       </c>
       <c r="B36">
-        <v>3.463794001834574</v>
+        <v>-5.162710744816398</v>
       </c>
       <c r="C36">
-        <v>-5.162710744816398</v>
-      </c>
-      <c r="D36">
-        <v>1.772180226664384</v>
-      </c>
-      <c r="E36">
-        <v>-2.913197352694598</v>
-      </c>
-      <c r="F36">
-        <v>0.003577484285359203</v>
-      </c>
-      <c r="G36">
         <v>0.01194652643141162</v>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>methylesterase PCR A (PMEPCRA) | FUNCTIONS IN: enzyme inhibitor activity, pectinesterase activity | INVOLVED IN: cell wall modification | LOCATED IN: cell wall, plasma membrane, plant-type cell wall | EXPRESSED IN: 25 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Pectinesterase, active site , Pectin lyase fold/virulence factor , Pectinesterase inhibitor , Pectinesterase, catalytic , Pectin lyase fold | BEST Arabidopsis thaliana protein match is: Plant invertase/pectin methylesterase inhibitor superfamily</t>
         </is>
@@ -1456,24 +1016,12 @@
         </is>
       </c>
       <c r="B37">
-        <v>3.394730560358241</v>
+        <v>-5.151304797362302</v>
       </c>
       <c r="C37">
-        <v>-5.151304797362302</v>
-      </c>
-      <c r="D37">
-        <v>1.68571010957842</v>
-      </c>
-      <c r="E37">
-        <v>-3.055866348604029</v>
-      </c>
-      <c r="F37">
-        <v>0.002244112638999479</v>
-      </c>
-      <c r="G37">
         <v>0.007967820841260727</v>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -1486,24 +1034,12 @@
         </is>
       </c>
       <c r="B38">
-        <v>18.71183162774037</v>
+        <v>-5.137983488832703</v>
       </c>
       <c r="C38">
-        <v>-5.137983488832703</v>
-      </c>
-      <c r="D38">
-        <v>0.988785731407422</v>
-      </c>
-      <c r="E38">
-        <v>-5.196255695882038</v>
-      </c>
-      <c r="F38">
-        <v>2.033425246319079e-007</v>
-      </c>
-      <c r="G38">
         <v>1.846734005471067e-006</v>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>GroES-like zinc-binding dehydrogenase family protein | FUNCTIONS IN: oxidoreductase activity, zinc ion binding | INVOLVED IN: oxidation reduction | EXPRESSED IN: 12 plant structures | EXPRESSED DURING: LP.04 four leaves visible, 4 anthesis, LP.02 two leaves visible, petal differentiation and expansion stage, D bilateral stage | CONTAINS InterPro DOMAIN/s: GroES-like , Alcohol dehydrogenase GroES-like , Alcohol dehydrogenase, zinc-containing, conserved site , Alcohol dehydrogenase, C-terminal , Alcohol dehydrogenase superfamily, zinc-containing | BEST Arabidopsis thaliana protein match is: GroES-like zinc-binding dehydrogenase family protein</t>
         </is>
@@ -1516,24 +1052,12 @@
         </is>
       </c>
       <c r="B39">
-        <v>3.247303049488655</v>
+        <v>-5.069133064584385</v>
       </c>
       <c r="C39">
-        <v>-5.069133064584385</v>
-      </c>
-      <c r="D39">
-        <v>1.624735207016231</v>
-      </c>
-      <c r="E39">
-        <v>-3.119974899721456</v>
-      </c>
-      <c r="F39">
-        <v>0.001808664512016948</v>
-      </c>
-      <c r="G39">
         <v>0.006609360951720428</v>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -1546,24 +1070,12 @@
         </is>
       </c>
       <c r="B40">
-        <v>6.33391855605371</v>
+        <v>-5.02473469842786</v>
       </c>
       <c r="C40">
-        <v>-5.02473469842786</v>
-      </c>
-      <c r="D40">
-        <v>1.480434336001598</v>
-      </c>
-      <c r="E40">
-        <v>-3.394094946486323</v>
-      </c>
-      <c r="F40">
-        <v>0.000688558156365639</v>
-      </c>
-      <c r="G40">
         <v>0.002827836251808828</v>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -1576,24 +1088,12 @@
         </is>
       </c>
       <c r="B41">
-        <v>3.079892569264841</v>
+        <v>-5.011705714140923</v>
       </c>
       <c r="C41">
-        <v>-5.011705714140923</v>
-      </c>
-      <c r="D41">
-        <v>1.746917536375877</v>
-      </c>
-      <c r="E41">
-        <v>-2.868885113225273</v>
-      </c>
-      <c r="F41">
-        <v>0.004119213904516434</v>
-      </c>
-      <c r="G41">
         <v>0.01345032369054141</v>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>hypothetical protein</t>
         </is>
@@ -1606,24 +1106,12 @@
         </is>
       </c>
       <c r="B42">
-        <v>3.107695197317897</v>
+        <v>-5.004775303140024</v>
       </c>
       <c r="C42">
-        <v>-5.004775303140024</v>
-      </c>
-      <c r="D42">
-        <v>1.668158539246366</v>
-      </c>
-      <c r="E42">
-        <v>-3.000179650431224</v>
-      </c>
-      <c r="F42">
-        <v>0.002698204125339143</v>
-      </c>
-      <c r="G42">
         <v>0.00937688603461561</v>
       </c>
-      <c r="H42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>member of SPL gene family, encodes DNA binding proteins and putative transcription factors. All have the SBP-box, which encodes the SBP-domain, required for and sufficient for interaction with DNA. | squamosa promoter binding protein-like 1 (SPL1) | FUNCTIONS IN: DNA binding, sequence-specific DNA binding transcription factor activity | INVOLVED IN: regulation of transcription | LOCATED IN: nucleus | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Transcription factor, SBP-box , Ankyrin repeat-containing domain , Ankyrin repeat | BEST Arabidopsis thaliana protein match is: squamosa promoter-binding protein-like 12</t>
         </is>
@@ -1636,24 +1124,12 @@
         </is>
       </c>
       <c r="B43">
-        <v>34.60751554713392</v>
+        <v>-5.0030512988696</v>
       </c>
       <c r="C43">
-        <v>-5.0030512988696</v>
-      </c>
-      <c r="D43">
-        <v>0.716195539808717</v>
-      </c>
-      <c r="E43">
-        <v>-6.985594046293315</v>
-      </c>
-      <c r="F43">
-        <v>2.83653172111332e-012</v>
-      </c>
-      <c r="G43">
         <v>5.008758836795708e-011</v>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>SAUR-like auxin-responsive protein family | CONTAINS InterPro DOMAIN/s: Auxin responsive SAUR protein | BEST Arabidopsis thaliana protein match is: SAUR-like auxin-responsive protein family</t>
         </is>
@@ -1666,24 +1142,12 @@
         </is>
       </c>
       <c r="B44">
-        <v>3.096932212281193</v>
+        <v>-5.002894642525647</v>
       </c>
       <c r="C44">
-        <v>-5.002894642525647</v>
-      </c>
-      <c r="D44">
-        <v>1.812329889520608</v>
-      </c>
-      <c r="E44">
-        <v>-2.760476815757311</v>
-      </c>
-      <c r="F44">
-        <v>0.00577170544373655</v>
-      </c>
-      <c r="G44">
         <v>0.01793818006077922</v>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Encodes a protein with similarity to the TAA1 trytophan aminotransferase involved in IAA biosynthesis. Double mutant analyses suggest that this protein is involved in regulating many aspects of plant growth and development from embryogenesis to flower formation and plays a role in ethylene-mediated signaling. | tryptophan aminotransferase related 2 (TAR2) | FUNCTIONS IN: L-tryptophan:2-oxoglutarate aminotransferase activity, carbon-sulfur lyase activity, L-tryptophan:pyruvate aminotransferase activity | INVOLVED IN: in 12 processes | LOCATED IN: endomembrane system | EXPRESSED IN: 21 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Pyridoxal phosphate-dependent transferase, major domain , Pyridoxal phosphate-dependent transferase, major region, subdomain 1 , Allinase, C-terminal | BEST Arabidopsis thaliana protein match is: tryptophan aminotransferase related 1</t>
         </is>
@@ -1696,24 +1160,12 @@
         </is>
       </c>
       <c r="B45">
-        <v>649.1794310660448</v>
+        <v>-4.99049064094528</v>
       </c>
       <c r="C45">
-        <v>-4.99049064094528</v>
-      </c>
-      <c r="D45">
-        <v>0.3475823699316629</v>
-      </c>
-      <c r="E45">
-        <v>-14.35772085312165</v>
-      </c>
-      <c r="F45">
-        <v>9.531028443330976e-047</v>
-      </c>
-      <c r="G45">
         <v>2.043634041649082e-044</v>
       </c>
-      <c r="H45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Leucine-rich repeat (LRR) family protein | INVOLVED IN: signal transduction, defense response | LOCATED IN: apoplast, cell wall, chloroplast, membrane | EXPRESSED IN: 23 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Leucine-rich repeat-containing N-terminal domain, type 2 , Leucine-rich repeat | BEST Arabidopsis thaliana protein match is: Leucine-rich repeat (LRR) family protein</t>
         </is>
@@ -1726,24 +1178,12 @@
         </is>
       </c>
       <c r="B46">
-        <v>3.061309925529308</v>
+        <v>-4.987327528736861</v>
       </c>
       <c r="C46">
-        <v>-4.987327528736861</v>
-      </c>
-      <c r="D46">
-        <v>1.743107160709631</v>
-      </c>
-      <c r="E46">
-        <v>-2.861170925777441</v>
-      </c>
-      <c r="F46">
-        <v>0.004220794261790394</v>
-      </c>
-      <c r="G46">
         <v>0.0137282522406745</v>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Plant invertase/pectin methylesterase inhibitor superfamily protein | FUNCTIONS IN: enzyme inhibitor activity, pectinesterase inhibitor activity, pectinesterase activity | INVOLVED IN: biological_process unknown | LOCATED IN: cellular_component unknown | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Pectinesterase inhibitor | BEST Arabidopsis thaliana protein match is: Plant invertase/pectin methylesterase inhibitor superfamily protein</t>
         </is>
@@ -1756,24 +1196,12 @@
         </is>
       </c>
       <c r="B47">
-        <v>27.94641684611231</v>
+        <v>-4.966527587288146</v>
       </c>
       <c r="C47">
-        <v>-4.966527587288146</v>
-      </c>
-      <c r="D47">
-        <v>0.7679064229221098</v>
-      </c>
-      <c r="E47">
-        <v>-6.467620844202668</v>
-      </c>
-      <c r="F47">
-        <v>9.955791760900567e-011</v>
-      </c>
-      <c r="G47">
         <v>1.446094810999454e-009</v>
       </c>
-      <c r="H47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Encodes an aspartic proteinase that forms a heterodimer and is stable over a broad pH range (ph 3-8). | aspartic proteinase A1 (APA1) | FUNCTIONS IN: endopeptidase activity | INVOLVED IN: proteolysis, response to salt stress | LOCATED IN: vacuole | EXPRESSED IN: 25 plant structures | EXPRESSED DURING: 16 growth stages | CONTAINS InterPro DOMAIN/s: Saposin-like , Peptidase aspartic , Peptidase aspartic, catalytic , Saposin-like type B, 1 , Saposin-like type B, 2 , Saposin B , Peptidase A1 , Peptidase aspartic, active site | BEST Arabidopsis thaliana protein match is: Saposin-like aspartyl protease family protein</t>
         </is>
@@ -1786,24 +1214,12 @@
         </is>
       </c>
       <c r="B48">
-        <v>1133.895375921154</v>
+        <v>-4.961484092698271</v>
       </c>
       <c r="C48">
-        <v>-4.961484092698271</v>
-      </c>
-      <c r="D48">
-        <v>0.5272830913494239</v>
-      </c>
-      <c r="E48">
-        <v>-9.40952625657089</v>
-      </c>
-      <c r="F48">
-        <v>4.983780878897861e-021</v>
-      </c>
-      <c r="G48">
         <v>2.101214282912106e-019</v>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>GDSL-like Lipase/Acylhydrolase superfamily protein | FUNCTIONS IN: hydrolase activity, acting on ester bonds, carboxylesterase activity | INVOLVED IN: lipid metabolic process | LOCATED IN: endomembrane system | EXPRESSED IN: 15 plant structures | EXPRESSED DURING: 7 growth stages | CONTAINS InterPro DOMAIN/s: Lipase, GDSL | BEST Arabidopsis thaliana protein match is: Li-tolerant lipase 1</t>
         </is>
@@ -1816,24 +1232,12 @@
         </is>
       </c>
       <c r="B49">
-        <v>2.965206050310354</v>
+        <v>-4.946568143170397</v>
       </c>
       <c r="C49">
-        <v>-4.946568143170397</v>
-      </c>
-      <c r="D49">
-        <v>1.610332660914096</v>
-      </c>
-      <c r="E49">
-        <v>-3.071767879540185</v>
-      </c>
-      <c r="F49">
-        <v>0.002127951306465434</v>
-      </c>
-      <c r="G49">
         <v>0.007617855893427059</v>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>UDP-Glycosyltransferase superfamily protein | FUNCTIONS IN: UDP-glycosyltransferase activity, transferase activity, transferring glycosyl groups | INVOLVED IN: metabolic process | LOCATED IN: cellular_component unknown | EXPRESSED IN: root | CONTAINS InterPro DOMAIN/s: UDP-glucuronosyl/UDP-glucosyltransferase | BEST Arabidopsis thaliana protein match is: UDP-Glycosyltransferase superfamily protein</t>
         </is>
@@ -1846,24 +1250,12 @@
         </is>
       </c>
       <c r="B50">
-        <v>2.965206050310354</v>
+        <v>-4.946568143170397</v>
       </c>
       <c r="C50">
-        <v>-4.946568143170397</v>
-      </c>
-      <c r="D50">
-        <v>1.610332660914096</v>
-      </c>
-      <c r="E50">
-        <v>-3.071767879540185</v>
-      </c>
-      <c r="F50">
-        <v>0.002127951306465434</v>
-      </c>
-      <c r="G50">
         <v>0.007617855893427059</v>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>Remorin family protein | CONTAINS InterPro DOMAIN/s: Remorin, C-terminal | BEST Arabidopsis thaliana protein match is: Remorin family protein</t>
         </is>
@@ -1876,26 +1268,914 @@
         </is>
       </c>
       <c r="B51">
-        <v>2.970906608482835</v>
+        <v>-4.940519359357293</v>
       </c>
       <c r="C51">
-        <v>-4.940519359357293</v>
-      </c>
-      <c r="D51">
-        <v>1.808034875958025</v>
-      </c>
-      <c r="E51">
-        <v>-2.732535431176048</v>
-      </c>
-      <c r="F51">
-        <v>0.006284891122718447</v>
-      </c>
-      <c r="G51">
         <v>0.01929606419431108</v>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>RING/U-box superfamily protein | FUNCTIONS IN: zinc ion binding | CONTAINS InterPro DOMAIN/s: Zinc finger, RING-type , Zinc finger, C3HC4 RING-type | BEST Arabidopsis thaliana protein match is: RING/U-box superfamily protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Sopen06g003960</t>
+        </is>
+      </c>
+      <c r="B52">
+        <v>-4.940152662570001</v>
+      </c>
+      <c r="C52">
+        <v>8.775229202073079e-056</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Plant invertase/pectin methylesterase inhibitor superfamily | FUNCTIONS IN: enzyme inhibitor activity, pectinesterase activity | INVOLVED IN: cell wall modification | LOCATED IN: endomembrane system, cell wall, plant-type cell wall | EXPRESSED IN: flower | CONTAINS InterPro DOMAIN/s: Pectinesterase, active site , Pectin lyase fold/virulence factor , Pectinesterase, catalytic , Pectinesterase inhibitor , Pectin lyase fold | BEST Arabidopsis thaliana protein match is: Plant invertase/pectin methylesterase inhibitor superfamily</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Sopen07g005610</t>
+        </is>
+      </c>
+      <c r="B53">
+        <v>-4.922587974125922</v>
+      </c>
+      <c r="C53">
+        <v>0.003932396579349532</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Encodes a secretory phospholipase A2 enzyme, which specifically hydrolyzes the sn-2 position of phospholipids. The enzyme has a preference towards linoleoyl acyl chain over palmitoyl acyl chain. It also has a slight preference for phosphatidylcholine over phosphatidylethanolamine. | PLA2-ALPHA | FUNCTIONS IN: phospholipase A2 activity | INVOLVED IN: phospholipid metabolic process, lipid catabolic process | LOCATED IN: vacuole | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Phospholipase A2 , Phospholipase A2, active site , Phospholipase A2, eukaryotic | BEST Arabidopsis thaliana protein match is: Phospholipase A2 family protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Sopen10g017470</t>
+        </is>
+      </c>
+      <c r="B54">
+        <v>-4.878095345572995</v>
+      </c>
+      <c r="C54">
+        <v>4.102676225489338e-030</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Annexin-like protein RJ4 - Fragaria ananassa (Strawberry), annexin 8 (ANNAT8) | FUNCTIONS IN: calcium-dependent phospholipid binding, calcium ion binding | INVOLVED IN: response to water deprivation, response to salt stress, response to cold, response to heat | EXPRESSED IN: embryo, pedicel, synergid | EXPRESSED DURING: 4 anthesis, C globular stage | CONTAINS InterPro DOMAIN/s: Annexin like protein , Annexin repeat , Annexin repeat, conserved site , Annexin , Annexin, type plant | BEST Arabidopsis thaliana protein match is: annexin 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Sopen02g019820</t>
+        </is>
+      </c>
+      <c r="B55">
+        <v>-4.832687109405506</v>
+      </c>
+      <c r="C55">
+        <v>4.845272153662437e-025</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Sopen02g020630</t>
+        </is>
+      </c>
+      <c r="B56">
+        <v>-4.832671579056385</v>
+      </c>
+      <c r="C56">
+        <v>1.288194997174587e-011</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>GDSL-like Lipase/Acylhydrolase superfamily protein | FUNCTIONS IN: hydrolase activity, acting on ester bonds, carboxylesterase activity | INVOLVED IN: lipid metabolic process | LOCATED IN: endomembrane system | EXPRESSED IN: 19 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Lipase, GDSL | BEST Arabidopsis thaliana protein match is: GDSL-like Lipase/Acylhydrolase superfamily protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Sopen09g035630</t>
+        </is>
+      </c>
+      <c r="B57">
+        <v>-4.817150616083603</v>
+      </c>
+      <c r="C57">
+        <v>0.01273737909274257</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Sopen04g030010</t>
+        </is>
+      </c>
+      <c r="B58">
+        <v>-4.795740076878582</v>
+      </c>
+      <c r="C58">
+        <v>0.0003455029433943533</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Eukaryotic aspartyl protease family protein | FUNCTIONS IN: aspartic-type endopeptidase activity | INVOLVED IN: proteolysis | LOCATED IN: apoplast, cell wall, plant-type cell wall | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 14 growth stages | CONTAINS InterPro DOMAIN/s: Peptidase aspartic , Peptidase aspartic, catalytic , Peptidase A1 | BEST Arabidopsis thaliana protein match is: Eukaryotic aspartyl protease family protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Sopen04g001870</t>
+        </is>
+      </c>
+      <c r="B59">
+        <v>-4.795737315329864</v>
+      </c>
+      <c r="C59">
+        <v>2.824314041204652e-014</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>encodes a cytosolic thioredoxin that reduces disulfide bridges of target proteins by the reversible formation of a disulfide bridge between two neighboring Cys residues present in the active site. Thioredoxins have been found to regulate a variety of biological reactions in prokaryotic and eukaryotic cells. | thioredoxin 2 (TRX2) | FUNCTIONS IN: oxidoreductase activity, acting on sulfur group of donors, disulfide as acceptor | INVOLVED IN: N-terminal protein myristoylation, sulfate assimilation | LOCATED IN: cytosol, plasma membrane | EXPRESSED IN: 24 plant structures | EXPRESSED DURING: 15 growth stages | CONTAINS InterPro DOMAIN/s: Thioredoxin fold , Thioredoxin, core , Thioredoxin domain , Thioredoxin, conserved site , Thioredoxin-like subdomain , Thioredoxin-like , Thioredoxin-like fold | BEST Arabidopsis thaliana protein match is: thioredoxin H-type 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Sopen11g001400</t>
+        </is>
+      </c>
+      <c r="B60">
+        <v>-4.793840548164823</v>
+      </c>
+      <c r="C60">
+        <v>0.01364122128355096</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>unknown protein | FUNCTIONS IN: molecular_function unknown | INVOLVED IN: biological_process unknown | LOCATED IN: plasma membrane | EXPRESSED IN: 17 plant structures | EXPRESSED DURING: 12 growth stages</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Sopen05g018270</t>
+        </is>
+      </c>
+      <c r="B61">
+        <v>-4.765313714689557</v>
+      </c>
+      <c r="C61">
+        <v>0.02071197333559727</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Sopen03g014380</t>
+        </is>
+      </c>
+      <c r="B62">
+        <v>-4.747450689867933</v>
+      </c>
+      <c r="C62">
+        <v>0.01747671517242334</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Reverse transcriptase, RNA-dependent DNA polymerase, Retrovirus-related Pol polyprotein from transposon TNT 1-94 | Reverse transcriptase (EC 2.7.7.49) | Endonuclease) - Nicotiana tabacum (Common tobacco), Encodes a cysteine-rich receptor-like protein kinase. | cysteine-rich RLK (RECEPTOR-like protein kinase) 8 (CRK8) | FUNCTIONS IN: kinase activity | INVOLVED IN: protein amino acid phosphorylation | CONTAINS InterPro DOMAIN/s: Protein kinase, ATP binding site , Reverse transcriptase, RNA-dependent DNA polymerase , Serine/threonine-protein kinase domain , Protein of unknown function DUF26 , Serine/threonine-protein kinase-like domain , Serine/threonine-protein kinase, active site , Protein kinase-like domain , Protein kinase, catalytic domain , Tyrosine-protein kinase, catalytic domain | BEST Arabidopsis thaliana protein match is: cysteine-rich RLK (RECEPTOR-like protein kinase) 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Sopen05g027290</t>
+        </is>
+      </c>
+      <c r="B63">
+        <v>-4.730619341216252</v>
+      </c>
+      <c r="C63">
+        <v>0.02150219364166039</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>B-box type zinc finger protein with CCT domain | FUNCTIONS IN: sequence-specific DNA binding transcription factor activity, zinc ion binding | INVOLVED IN: regulation of transcription | LOCATED IN: intracellular | CONTAINS InterPro DOMAIN/s: CCT domain , Zinc finger, B-box | BEST Arabidopsis thaliana protein match is: B-box type zinc finger protein with CCT domain</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Sopen03g035840</t>
+        </is>
+      </c>
+      <c r="B64">
+        <v>-4.708993171223253</v>
+      </c>
+      <c r="C64">
+        <v>0.006643492775372417</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Encodes a cinnamoyl CoA reductase. Involved in lignin biosynthesis. | cinnamoyl coa reductase 1 (CCR1) | CONTAINS InterPro DOMAIN/s: NAD-dependent epimerase/dehydratase , NAD(P)-binding domain | BEST Arabidopsis thaliana protein match is: cinnamoyl coa reductase</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Sopen02g035610</t>
+        </is>
+      </c>
+      <c r="B65">
+        <v>-4.707969471713007</v>
+      </c>
+      <c r="C65">
+        <v>7.025433568515501e-013</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Member of a diversely expressed predicted peptide family showing sequence similarity to tobacco Rapid Alkalinization Factor (RALF), and is believed to play an essential role in the physiology of Arabidopsis. Consists of a single exon and is characterized by a conserved C-terminal motif and N-terminal signal peptide. | ralf-like 34 (RALFL34) | CONTAINS InterPro DOMAIN/s: Rapid ALkalinization Factor | BEST Arabidopsis thaliana protein match is: rapid alkalinization factor 23</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Sopen10g029990</t>
+        </is>
+      </c>
+      <c r="B66">
+        <v>-4.701913475786545</v>
+      </c>
+      <c r="C66">
+        <v>2.855352427324717e-019</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Zeatin O-xylosyltransferase (EC 2.4.2.40) (Zeatin O-beta-D-xylosyltransferase) - Phaseolus vulgaris (Kidney bean) (French bean), UDP-glucosyl transferase 73B3 (UGT73B3) | FUNCTIONS IN: transferase activity, transferring hexosyl groups, quercetin 3-O-glucosyltransferase activity, UDP-glycosyltransferase activity, UDP-glucosyltransferase activity | INVOLVED IN: response to cyclopentenone, response to other organism | LOCATED IN: endomembrane system | CONTAINS InterPro DOMAIN/s: UDP-glucuronosyl/UDP-glucosyltransferase | BEST Arabidopsis thaliana protein match is: UDP-glucosyltransferase 73B2</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Sopen09g036220</t>
+        </is>
+      </c>
+      <c r="B67">
+        <v>-4.692826322407678</v>
+      </c>
+      <c r="C67">
+        <v>3.412628784719271e-010</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Leucine-rich receptor-like protein kinase family protein | FUNCTIONS IN: protein serine/threonine kinase activity, kinase activity, ATP binding | INVOLVED IN: transmembrane receptor protein tyrosine kinase signaling pathway, protein amino acid phosphorylation | LOCATED IN: endomembrane system | EXPRESSED IN: 23 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Protein kinase, ATP binding site , Protein kinase, catalytic domain , Leucine-rich repeat-containing N-terminal domain, type 2 , Leucine-rich repeat , Serine/threonine-protein kinase-like domain , Protein kinase-like domain | BEST Arabidopsis thaliana protein match is: Leucine-rich repeat protein kinase family protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Sopen01g051350</t>
+        </is>
+      </c>
+      <c r="B68">
+        <v>-4.691775562600634</v>
+      </c>
+      <c r="C68">
+        <v>0.01222985425619605</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Encodes a member of the cytochrome p450 CYP74 gene family that functions as an allene oxide synthase. This enzyme catalyzes dehydration of the hydroperoxide to an unstable allene oxide in the JA biosynthetic pathway. It shows a dual catalytic activity, the major one being a 13-AOS but also expressing a 9-AOS activity. | allene oxide synthase (AOS) | FUNCTIONS IN: hydro-lyase activity, allene oxide synthase activity, oxygen binding | INVOLVED IN: in 7 processes | LOCATED IN: in 7 components | EXPRESSED IN: 23 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Cytochrome P450 | BEST Arabidopsis thaliana protein match is: hydroperoxide lyase 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Sopen01g037300</t>
+        </is>
+      </c>
+      <c r="B69">
+        <v>-4.670676520028771</v>
+      </c>
+      <c r="C69">
+        <v>2.227747973048871e-047</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>FASCICLIN-like arabinogalactan-protein 10 (FLA10) | LOCATED IN: anchored to plasma membrane, plasma membrane, anchored to membrane | EXPRESSED IN: 17 plant structures | EXPRESSED DURING: 8 growth stages | CONTAINS InterPro DOMAIN/s: FAS1 domain | BEST Arabidopsis thaliana protein match is: FASCICLIN-like arabinogalactan protein 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Sopen02g021020</t>
+        </is>
+      </c>
+      <c r="B70">
+        <v>-4.667191104510953</v>
+      </c>
+      <c r="C70">
+        <v>0.004583702486073009</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>unknown protein | FUNCTIONS IN: molecular_function unknown | INVOLVED IN: biological_process unknown | LOCATED IN: endomembrane system | BEST Arabidopsis thaliana protein match is: unknown protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Sopen08g021860</t>
+        </is>
+      </c>
+      <c r="B71">
+        <v>-4.664088295501871</v>
+      </c>
+      <c r="C71">
+        <v>1.28283897688991e-014</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Sopen08g001930</t>
+        </is>
+      </c>
+      <c r="B72">
+        <v>-4.643358868010612</v>
+      </c>
+      <c r="C72">
+        <v>5.953076933953605e-016</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Bifunctional inhibitor/lipid-transfer protein/seed storage 2S albumin superfamily protein | FUNCTIONS IN: lipid binding | INVOLVED IN: lipid transport | LOCATED IN: chloroplast thylakoid membrane | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Bifunctional inhibitor/plant lipid transfer protein/seed storage , Plant lipid transfer protein/seed storage/trypsin-alpha amylase inhibitor , Plant lipid transfer protein/hydrophobic protein, helical domain | BEST Arabidopsis thaliana protein match is: Bifunctional inhibitor/lipid-transfer protein/seed storage 2S albumin superfamily protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Sopen09g030340</t>
+        </is>
+      </c>
+      <c r="B73">
+        <v>-4.637566533216411</v>
+      </c>
+      <c r="C73">
+        <v>0.02054387023330613</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Encodes a gene similar to cellulose synthase. Knock-out mutant has reduced growth, reduced xylan level and reduced xylan synthase activity in stems. | cellulose synthase-like D5 (CSLD5) | CONTAINS InterPro DOMAIN/s: Cellulose synthase | BEST Arabidopsis thaliana protein match is: cellulose synthase-like D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Sopen03g009060</t>
+        </is>
+      </c>
+      <c r="B74">
+        <v>-4.624489128588169</v>
+      </c>
+      <c r="C74">
+        <v>0.005540052172001522</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>RNA-directed DNA polymerase homolog (Reverse transcriptase homolog) - Oenothera bertiana (Berteros evening primrose), hypothetical protein | DNA/RNA polymerases superfamily protein.</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Sopen12g003970</t>
+        </is>
+      </c>
+      <c r="B75">
+        <v>-4.603112083715492</v>
+      </c>
+      <c r="C75">
+        <v>0.005244946788895494</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>long-chain acyl-CoA synthetase 8 (LACS8) | FUNCTIONS IN: long-chain fatty acid-CoA ligase activity, catalytic activity | INVOLVED IN: fatty acid biosynthetic process, metabolic process | LOCATED IN: endoplasmic reticulum | EXPRESSED IN: 23 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: AMP-binding, conserved site , AMP-dependent synthetase/ligase | BEST Arabidopsis thaliana protein match is: long chain acyl-CoA synthetase 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Sopen06g001570</t>
+        </is>
+      </c>
+      <c r="B76">
+        <v>-4.591189003210686</v>
+      </c>
+      <c r="C76">
+        <v>1.92562567681818e-010</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Sopen06g031050</t>
+        </is>
+      </c>
+      <c r="B77">
+        <v>-4.571836417705108</v>
+      </c>
+      <c r="C77">
+        <v>6.874624674767774e-045</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>encodes a beta-mannan synthase based on in vitro enzyme assays from heterologously expressed protein | cellulose synthase-like A02 (CSLA02) | CONTAINS InterPro DOMAIN/s: Glycosyl transferase, family 2 | BEST Arabidopsis thaliana protein match is: Nucleotide-diphospho-sugar transferases superfamily protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Sopen09g034690</t>
+        </is>
+      </c>
+      <c r="B78">
+        <v>-4.563671199803979</v>
+      </c>
+      <c r="C78">
+        <v>1.568463346465676e-007</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Sopen08g019010</t>
+        </is>
+      </c>
+      <c r="B79">
+        <v>-4.54591918327217</v>
+      </c>
+      <c r="C79">
+        <v>0.04888962660483989</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Encodes transcription factor involved in photomorphogenesis. Regulates gibberellin biosynthesis. Activated by AGAMOUS in a cal-1, ap1-1 background. Expressed at low levels in developing stamens. Increased levels of ATH1 severely delay flowering in the C24 accession. Most remarkably, ectopically expressed ATH1 hardly had an effect on flowering time in the Col-0 and Ler accessions. ATH1 physically interacts with STM, BP and KNAT6 and enhances the shoot apical meristem defect of some of these genes suggesting a role in SAM maintenance. Nuclear localization is dependent upon interaction with STM. | homeobox gene 1 (ATH1) | CONTAINS InterPro DOMAIN/s: Homeobox , Homeodomain-like , POX , Homeodomain-related | BEST Arabidopsis thaliana protein match is: BEL1-like homeodomain 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Sopen01g043160</t>
+        </is>
+      </c>
+      <c r="B80">
+        <v>-4.52512873512003</v>
+      </c>
+      <c r="C80">
+        <v>2.531275703001587e-007</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Actin-binding FH2 (formin homology 2) family protein | FUNCTIONS IN: actin binding | INVOLVED IN: cellular component organization, actin cytoskeleton organization | LOCATED IN: endomembrane system | EXPRESSED IN: 20 plant structures | EXPRESSED DURING: 11 growth stages | CONTAINS InterPro DOMAIN/s: Actin-binding FH2/DRF autoregulatory , Actin-binding FH2 | BEST Arabidopsis thaliana protein match is: formin homolog 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Sopen03g039910</t>
+        </is>
+      </c>
+      <c r="B81">
+        <v>-4.523284719953027</v>
+      </c>
+      <c r="C81">
+        <v>0.03339093897968588</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Sopen02g035710</t>
+        </is>
+      </c>
+      <c r="B82">
+        <v>-4.514412958055347</v>
+      </c>
+      <c r="C82">
+        <v>0.01996962000141256</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>MATE efflux family protein | FUNCTIONS IN: antiporter activity, drug transmembrane transporter activity, transporter activity | INVOLVED IN: drug transmembrane transport, transmembrane transport | LOCATED IN: chloroplast, membrane | EXPRESSED IN: 17 plant structures | EXPRESSED DURING: 9 growth stages | CONTAINS InterPro DOMAIN/s: MATE family transporter related protein , Multi antimicrobial extrusion protein MatE | BEST Arabidopsis thaliana protein match is: MATE efflux family protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Sopen02g034520</t>
+        </is>
+      </c>
+      <c r="B83">
+        <v>-4.511902804020936</v>
+      </c>
+      <c r="C83">
+        <v>0.007755093361307281</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Encodes protein with TCP (TB1,CYC,PCF) domain which is likely to be involved in DNA binding and protein-protein interactions. Based on genome analysis, there is a 9-member gene family that possesses this domain in Arabidopsis. Orthologue of Antirrhinum gene CYCLOIDEA. | TCP1 | FUNCTIONS IN: DNA binding, sequence-specific DNA binding transcription factor activity | INVOLVED IN: flower development | LOCATED IN: cellular_component unknown | EXPRESSED IN: floral meristem | EXPRESSED DURING: 1 floral meristem visible, 2 floral meristem notched | CONTAINS InterPro DOMAIN/s: Transcription factor, TCP , CYC/TB1, R domain , Transcription factor TCP subgroup | BEST Arabidopsis thaliana protein match is: TCP domain protein 12</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Sopen01g036250</t>
+        </is>
+      </c>
+      <c r="B84">
+        <v>-4.510196345320502</v>
+      </c>
+      <c r="C84">
+        <v>0.0007906950160729233</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Encodes a homeodomain-leucine zipper protein that is rapidly and strongly induced by changes in the ratio of red to far-red light. It is also involved in cell expansion and cell proliferation and in the response to auxin. | homeobox protein 2 (HB-2) | CONTAINS InterPro DOMAIN/s: HD-ZIP protein, N-terminal , Helix-turn-helix motif, lambda-like repressor , Homeobox , Homeobox, conserved site , Homeodomain-like , Leucine zipper, homeobox-associated , Homeodomain-related | BEST Arabidopsis thaliana protein match is: Homeobox-leucine zipper protein 4 (HB-4) / HD-ZIP protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Sopen04g032170</t>
+        </is>
+      </c>
+      <c r="B85">
+        <v>-4.472613875103113</v>
+      </c>
+      <c r="C85">
+        <v>5.790581499264484e-032</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Leucine-rich repeat protein kinase family protein | FUNCTIONS IN: protein serine/threonine kinase activity, kinase activity, ATP binding | INVOLVED IN: transmembrane receptor protein tyrosine kinase signaling pathway, protein amino acid phosphorylation | LOCATED IN: endomembrane system | EXPRESSED IN: 21 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Protein kinase, catalytic domain , Leucine-rich repeat , Serine/threonine-protein kinase-like domain , Protein kinase-like domain | BEST Arabidopsis thaliana protein match is: Leucine-rich repeat protein kinase family protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Sopen08g022640</t>
+        </is>
+      </c>
+      <c r="B86">
+        <v>-4.472005628428673</v>
+      </c>
+      <c r="C86">
+        <v>7.330495520550434e-084</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>CAP (Cysteine-rich secretory proteins, Antigen 5, and Pathogenesis-related 1 protein) superfamily protein | FUNCTIONS IN: molecular_function unknown | INVOLVED IN: biological_process unknown | LOCATED IN: endomembrane system, extracellular region | EXPRESSED IN: root | CONTAINS InterPro DOMAIN/s: Allergen V5/Tpx-1 related, conserved site , Allergen V5/Tpx-1 related , Ves allergen , SCP-like extracellular | BEST Arabidopsis thaliana protein match is: CAP (Cysteine-rich secretory proteins, Antigen 5, and Pathogenesis-related 1 protein) superfamily protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Sopen04g021640</t>
+        </is>
+      </c>
+      <c r="B87">
+        <v>-4.462512381549101</v>
+      </c>
+      <c r="C87">
+        <v>6.609623336651711e-005</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>GDSL-like Lipase/Acylhydrolase superfamily protein | FUNCTIONS IN: hydrolase activity, acting on ester bonds, carboxylesterase activity | INVOLVED IN: lipid metabolic process | LOCATED IN: endomembrane system | EXPRESSED IN: 15 plant structures | EXPRESSED DURING: 7 growth stages | CONTAINS InterPro DOMAIN/s: Lipase, GDSL | BEST Arabidopsis thaliana protein match is: Li-tolerant lipase 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Sopen06g025810</t>
+        </is>
+      </c>
+      <c r="B88">
+        <v>-4.455155996416218</v>
+      </c>
+      <c r="C88">
+        <v>0.008482216239229637</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Eukaryotic aspartyl protease family protein | FUNCTIONS IN: aspartic-type endopeptidase activity | INVOLVED IN: proteolysis | LOCATED IN: apoplast | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Peptidase aspartic , Peptidase aspartic, catalytic , Peptidase A1 , Peptidase aspartic, active site | BEST Arabidopsis thaliana protein match is: Eukaryotic aspartyl protease family protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Sopen04g027790</t>
+        </is>
+      </c>
+      <c r="B89">
+        <v>-4.447016569659681</v>
+      </c>
+      <c r="C89">
+        <v>0.008727636317719943</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Required for flavonoid 3 hydroxylase activity. | TRANSPARENT TESTA 7 (TT7) | CONTAINS InterPro DOMAIN/s: Cytochrome P450 , Cytochrome P450, E-class, group I , Cytochrome P450, conserved site | BEST Arabidopsis thaliana protein match is: cytochrome P450, family 706, subfamily A, polypeptide 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Sopen08g022400</t>
+        </is>
+      </c>
+      <c r="B90">
+        <v>-4.441288870406201</v>
+      </c>
+      <c r="C90">
+        <v>0.02995451005722768</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>embryo defective 1075 (emb1075) | FUNCTIONS IN: pyridoxal phosphate binding, carboxy-lyase activity, catalytic activity | INVOLVED IN: cellular amino acid metabolic process, embryo development ending in seed dormancy | LOCATED IN: cellular_component unknown | EXPRESSED IN: 25 plant structures | EXPRESSED DURING: 15 growth stages | CONTAINS InterPro DOMAIN/s: Pyridoxal phosphate-dependent transferase, major domain , Pyridoxal phosphate-dependent decarboxylase , Pyridoxal-phosphate binding site , Pyridoxal phosphate-dependent transferase, major region, subdomain 1 | BEST Arabidopsis thaliana protein match is: glutamate decarboxylase 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Sopen03g034760</t>
+        </is>
+      </c>
+      <c r="B91">
+        <v>-4.437156479273109</v>
+      </c>
+      <c r="C91">
+        <v>0.000102705638482723</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Polynucleotidyl transferase, ribonuclease H-like superfamily protein | FUNCTIONS IN: exonuclease activity, nucleic acid binding | INVOLVED IN: biological_process unknown | LOCATED IN: intracellular | EXPRESSED IN: 23 plant structures | EXPRESSED DURING: 13 growth stages | CONTAINS InterPro DOMAIN/s: Exonuclease , Polynucleotidyl transferase, ribonuclease H fold , Exonuclease, RNase T/DNA polymerase III | BEST Arabidopsis thaliana protein match is: Polynucleotidyl transferase, ribonuclease H-like superfamily protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Sopen01g004960</t>
+        </is>
+      </c>
+      <c r="B92">
+        <v>-4.434623313647417</v>
+      </c>
+      <c r="C92">
+        <v>5.372755956091145e-006</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Encodes a member of the DREB subfamily A-1 of ERF/AP2 transcription factor family (CBF2). The protein contains one AP2 domain. There are six members in this subfamily, including CBF1, CBF2, and CBF3. This gene is involved in response to low temperature, abscisic acid, and circadian rhythm. Overexpressing this gene leads to increased freeze tolerance and induces the expression level of 85 cold-induced genes and reduces the expression level of 8 cold-repressed genes, which constitute the CBF2 regulon. Mutations in CBF2 increases the expression level of CBF1 and CBF3, suggesting that this gene may be involved in a negative regulatory or feedback circuit of the CBF pathway. | C-repeat/DRE binding factor 2 (CBF2) | CONTAINS InterPro DOMAIN/s: DNA-binding, integrase-type , Pathogenesis-related transcriptional factor/ERF, DNA-binding | BEST Arabidopsis thaliana protein match is: C-repeat/DRE binding factor 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Sopen12g023740</t>
+        </is>
+      </c>
+      <c r="B93">
+        <v>-4.425546008222123</v>
+      </c>
+      <c r="C93">
+        <v>1.195562123350358e-005</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Sopen03g030810</t>
+        </is>
+      </c>
+      <c r="B94">
+        <v>-4.416972195781817</v>
+      </c>
+      <c r="C94">
+        <v>8.091272581447373e-051</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Pectin lyase-like superfamily protein | CONTAINS InterPro DOMAIN/s: Pectin lyase fold/virulence factor , AmbAllergen , Pectate lyase/Amb allergen , Pectin lyase fold | BEST Arabidopsis thaliana protein match is: Pectin lyase-like superfamily protein ., Pectate lyase precursor (EC 4.2.2.2) - Lilium longiflorum (Trumpet lily), Pectin lyase fold</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Sopen12g030250</t>
+        </is>
+      </c>
+      <c r="B95">
+        <v>-4.392597045356278</v>
+      </c>
+      <c r="C95">
+        <v>0.0377788306105961</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Sopen01g038530</t>
+        </is>
+      </c>
+      <c r="B96">
+        <v>-4.385871811444424</v>
+      </c>
+      <c r="C96">
+        <v>1.258159373228389e-005</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Encodes a member of the CYP86A subfamily of cytochrome p450 genes. Expressed at moderate levels in flowers, leaves, roots and stems. | cytochrome P450, family 86, subfamily A, polypeptide 2 (CYP86A2) | CONTAINS InterPro DOMAIN/s: Cytochrome P450 , Cytochrome P450, E-class, group I , Cytochrome P450, conserved site | BEST Arabidopsis thaliana protein match is: cytochrome P450, family 86, subfamily A, polypeptide 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Sopen10g009540</t>
+        </is>
+      </c>
+      <c r="B97">
+        <v>-4.370848746707801</v>
+      </c>
+      <c r="C97">
+        <v>0.04387268956089468</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>member of MRP subfamily | multidrug resistance-associated protein 9 (MRP9) | FUNCTIONS IN: ATPase activity, coupled to transmembrane movement of substances | INVOLVED IN: response to nematode | LOCATED IN: integral to membrane | EXPRESSED IN: root | CONTAINS InterPro DOMAIN/s: ATPase, AAA+ type, core , ABC transporter-like , ABC transporter, transmembrane domain, type 1 , ABC transporter integral membrane type 1 , ABC transporter, transmembrane domain , ABC transporter, conserved site | BEST Arabidopsis thaliana protein match is: multidrug resistance-associated protein 15</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Sopen03g005370</t>
+        </is>
+      </c>
+      <c r="B98">
+        <v>-4.368413345724739</v>
+      </c>
+      <c r="C98">
+        <v>0.01146294069066729</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Sopen01g039470</t>
+        </is>
+      </c>
+      <c r="B99">
+        <v>-4.350677995039137</v>
+      </c>
+      <c r="C99">
+        <v>0.01301719710950802</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>hypothetical protein</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Sopen10g024760</t>
+        </is>
+      </c>
+      <c r="B100">
+        <v>-4.34736755480452</v>
+      </c>
+      <c r="C100">
+        <v>6.848463531016466e-010</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Aquaporin-like, a member of the plasma membrane intrinsic protein subfamily PIP1. localizes to the plasma membrane and exhibits water transport activity in Xenopus oocyte. expressed ubiquitously and protein level decreases slightly during leaf development. | plasma membrane intrinsic protein 1C (PIP1C) | FUNCTIONS IN: water channel activity | INVOLVED IN: response to water deprivation, response to salt stress, transport, water transport | LOCATED IN: plasma membrane, membrane | EXPRESSED IN: 22 plant structures | EXPRESSED DURING: 14 growth stages | CONTAINS InterPro DOMAIN/s: Major intrinsic protein, conserved site , Aquaporin , Major intrinsic protein | BEST Arabidopsis thaliana protein match is: plasma membrane intrinsic protein 1, 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Sopen05g008600</t>
+        </is>
+      </c>
+      <c r="B101">
+        <v>-4.338814728622752</v>
+      </c>
+      <c r="C101">
+        <v>2.930855897094083e-022</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>GDSL-like Lipase/Acylhydrolase superfamily protein | FUNCTIONS IN: hydrolase activity, acting on ester bonds, carboxylesterase activity | INVOLVED IN: lipid metabolic process | LOCATED IN: endomembrane system | EXPRESSED IN: guard cell | CONTAINS InterPro DOMAIN/s: Lipase, GDSL | BEST Arabidopsis thaliana protein match is: alpha-fucosidase 1</t>
         </is>
       </c>
     </row>

</xml_diff>